<commit_message>
near final notebook and app
</commit_message>
<xml_diff>
--- a/results/model3/model3_df_results.xlsx
+++ b/results/model3/model3_df_results.xlsx
@@ -35,7 +35,7 @@
       <color rgb="00F1F1F1"/>
     </font>
   </fonts>
-  <fills count="16">
+  <fills count="14">
     <fill>
       <patternFill/>
     </fill>
@@ -49,22 +49,32 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="00E9F7E5"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="0078C679"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="0063BC6E"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="00309950"/>
+        <fgColor rgb="00BAE3B3"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="0075C477"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="002C944C"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00248C46"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="0000441B"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00004C1E"/>
       </patternFill>
     </fill>
     <fill>
@@ -74,42 +84,22 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="000A7633"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="0000441B"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="000D7836"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="00005E26"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="00006428"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="0000682A"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="00005B25"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="00006227"/>
+        <fgColor rgb="000C7735"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="0005712F"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00005924"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00004E1F"/>
       </patternFill>
     </fill>
   </fills>
@@ -132,7 +122,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="15">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf applyAlignment="1" borderId="1" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
@@ -164,19 +154,13 @@
     <xf applyAlignment="1" borderId="0" fillId="6" fontId="2" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
+    <xf applyAlignment="1" borderId="0" fillId="7" fontId="3" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf applyAlignment="1" borderId="0" fillId="8" fontId="3" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
     <xf applyAlignment="1" borderId="0" fillId="13" fontId="3" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="0" fillId="7" fontId="3" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="0" fillId="14" fontId="3" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="0" fillId="8" fontId="3" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="0" fillId="15" fontId="3" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
     <xf applyAlignment="1" borderId="0" fillId="9" fontId="3" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
@@ -517,13 +501,13 @@
         <v>-4</v>
       </c>
       <c r="C2" s="2" t="n">
-        <v>-17.5851</v>
+        <v>-30.0126</v>
       </c>
       <c r="D2" s="3" t="n">
-        <v>1.1758</v>
+        <v>1.5189</v>
       </c>
       <c r="E2" s="3" t="n">
-        <v>3.5914</v>
+        <v>4.685</v>
       </c>
     </row>
     <row r="3">
@@ -534,13 +518,13 @@
         <v>-3</v>
       </c>
       <c r="C3" s="2" t="n">
-        <v>-6.8363</v>
+        <v>-11.4739</v>
       </c>
       <c r="D3" s="4" t="n">
-        <v>1.1623</v>
+        <v>1.4664</v>
       </c>
       <c r="E3" s="5" t="n">
-        <v>2.7335</v>
+        <v>3.4766</v>
       </c>
     </row>
     <row r="4">
@@ -551,13 +535,13 @@
         <v>-2</v>
       </c>
       <c r="C4" s="2" t="n">
-        <v>-3.0135</v>
+        <v>-5.6612</v>
       </c>
       <c r="D4" s="6" t="n">
-        <v>1.1107</v>
+        <v>1.4309</v>
       </c>
       <c r="E4" s="7" t="n">
-        <v>2.6366</v>
+        <v>3.437</v>
       </c>
     </row>
     <row r="5">
@@ -568,13 +552,13 @@
         <v>-1</v>
       </c>
       <c r="C5" s="2" t="n">
-        <v>-1.5372</v>
+        <v>-3.0416</v>
       </c>
       <c r="D5" s="8" t="n">
-        <v>1.1036</v>
+        <v>1.3929</v>
       </c>
       <c r="E5" s="9" t="n">
-        <v>2.6592</v>
+        <v>3.3217</v>
       </c>
     </row>
     <row r="6">
@@ -585,13 +569,13 @@
         <v>0</v>
       </c>
       <c r="C6" s="2" t="n">
-        <v>-0.9547</v>
+        <v>-2.2067</v>
       </c>
       <c r="D6" s="10" t="n">
-        <v>1.0832</v>
-      </c>
-      <c r="E6" s="11" t="n">
-        <v>2.6701</v>
+        <v>1.3874</v>
+      </c>
+      <c r="E6" s="9" t="n">
+        <v>3.3197</v>
       </c>
     </row>
     <row r="7">
@@ -602,13 +586,13 @@
         <v>1</v>
       </c>
       <c r="C7" s="2" t="n">
-        <v>-0.8283</v>
-      </c>
-      <c r="D7" s="12" t="n">
-        <v>1.0518</v>
-      </c>
-      <c r="E7" s="13" t="n">
-        <v>2.6292</v>
+        <v>-1.9761</v>
+      </c>
+      <c r="D7" s="11" t="n">
+        <v>1.3419</v>
+      </c>
+      <c r="E7" s="12" t="n">
+        <v>3.2641</v>
       </c>
     </row>
     <row r="8">
@@ -619,13 +603,13 @@
         <v>2</v>
       </c>
       <c r="C8" s="2" t="n">
-        <v>-0.8108</v>
-      </c>
-      <c r="D8" s="14" t="n">
-        <v>1.0642</v>
-      </c>
-      <c r="E8" s="15" t="n">
-        <v>2.6501</v>
+        <v>-1.8975</v>
+      </c>
+      <c r="D8" s="12" t="n">
+        <v>1.3462</v>
+      </c>
+      <c r="E8" s="13" t="n">
+        <v>3.2768</v>
       </c>
     </row>
     <row r="9">
@@ -636,13 +620,13 @@
         <v>3</v>
       </c>
       <c r="C9" s="2" t="n">
-        <v>-0.6709000000000001</v>
-      </c>
-      <c r="D9" s="16" t="n">
-        <v>1.0425</v>
-      </c>
-      <c r="E9" s="16" t="n">
-        <v>2.5543</v>
+        <v>-1.8189</v>
+      </c>
+      <c r="D9" s="14" t="n">
+        <v>1.3541</v>
+      </c>
+      <c r="E9" s="11" t="n">
+        <v>3.2277</v>
       </c>
     </row>
   </sheetData>

</xml_diff>